<commit_message>
Added check for BLQ
</commit_message>
<xml_diff>
--- a/Testing/Testing/Test Case 2/test_data2_09062022.xlsx
+++ b/Testing/Testing/Test Case 2/test_data2_09062022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher.Wilson\Documents\bmrn-test\Testing\Testing\Test Case 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D693A89-1F27-474E-826E-1403C318329A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2AC458-F3B1-43BD-858B-56A3D1F6DC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="71">
   <si>
     <t>In cell B1, please record the label for your endpoint or biomarker with unit</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>Time5</t>
+  </si>
+  <si>
+    <t>Dose</t>
   </si>
 </sst>
 </file>
@@ -870,7 +873,7 @@
   <dimension ref="A1:K159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B159" sqref="B139:B159"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,7 +906,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>15</v>

</xml_diff>